<commit_message>
added lincs portal URLs
</commit_message>
<xml_diff>
--- a/src/ontology/Ontorat files/LINCS_Primary_Cells_2018Jan.xlsx
+++ b/src/ontology/Ontorat files/LINCS_Primary_Cells_2018Jan.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Primary_Cells_20171127" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="283">
   <si>
     <t>pc_lincs_id</t>
   </si>
@@ -680,6 +680,189 @@
   </si>
   <si>
     <t>Daniel Cooper, Oliver He</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1021</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1001</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1002</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1003</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1004</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1005</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1006</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1007</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1008</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1009</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1010</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1011</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1012</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1013</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1014</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1015</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1016</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1017</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1018</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1019</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1020</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1022</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1023</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1024</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1025</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1026</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1027</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1028</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1029</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1030</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1031</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1032</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1033</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1034</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1035</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1036</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1037</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1038</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1039</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1040</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1041</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1042</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1043</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1044</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1045</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1046</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1047</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1048</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1049</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1050</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1051</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1052</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1053</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1054</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1055</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1056</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1057</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1058</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1059</t>
+  </si>
+  <si>
+    <t>http://lincsportal.ccs.miami.edu/cells/#/view/LPC-1060</t>
+  </si>
+  <si>
+    <t>LINCS protal URL</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,9 +1712,10 @@
     <col min="15" max="15" width="157.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="95.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1583,8 +1767,11 @@
       <c r="Q1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1624,8 +1811,11 @@
       <c r="Q2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -1665,8 +1855,11 @@
       <c r="Q3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -1706,8 +1899,11 @@
       <c r="Q4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -1747,8 +1943,11 @@
       <c r="Q5" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -1788,8 +1987,11 @@
       <c r="Q6" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>184</v>
       </c>
@@ -1829,8 +2031,11 @@
       <c r="Q7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>198</v>
       </c>
@@ -1858,8 +2063,11 @@
       <c r="Q8" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -1887,8 +2095,11 @@
       <c r="Q9" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>207</v>
       </c>
@@ -1916,8 +2127,11 @@
       <c r="Q10" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1954,8 +2168,11 @@
       <c r="Q11" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -1992,8 +2209,11 @@
       <c r="Q12" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -2030,8 +2250,11 @@
       <c r="Q13" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -2068,8 +2291,11 @@
       <c r="Q14" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>202</v>
       </c>
@@ -2118,8 +2344,11 @@
       <c r="Q15" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -2165,8 +2394,11 @@
       <c r="Q16" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -2212,8 +2444,11 @@
       <c r="Q17" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2253,8 +2488,11 @@
       <c r="Q18" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -2279,8 +2517,11 @@
       <c r="Q19" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -2320,8 +2561,11 @@
       <c r="Q20" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>150</v>
       </c>
@@ -2361,8 +2605,11 @@
       <c r="Q21" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>156</v>
       </c>
@@ -2408,8 +2655,11 @@
       <c r="Q22" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R22" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -2449,8 +2699,11 @@
       <c r="Q23" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -2502,8 +2755,11 @@
       <c r="Q24" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>192</v>
       </c>
@@ -2543,8 +2799,11 @@
       <c r="Q25" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>148</v>
       </c>
@@ -2584,8 +2843,11 @@
       <c r="Q26" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2625,8 +2887,11 @@
       <c r="Q27" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R27" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>170</v>
       </c>
@@ -2666,8 +2931,11 @@
       <c r="Q28" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -2707,8 +2975,11 @@
       <c r="Q29" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2748,8 +3019,11 @@
       <c r="Q30" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -2789,8 +3063,11 @@
       <c r="Q31" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R31" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -2830,8 +3107,11 @@
       <c r="Q32" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R32" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>200</v>
       </c>
@@ -2871,8 +3151,11 @@
       <c r="Q33" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R33" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -2912,8 +3195,11 @@
       <c r="Q34" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R34" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -2953,8 +3239,11 @@
       <c r="Q35" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2994,8 +3283,11 @@
       <c r="Q36" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R36" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -3035,8 +3327,11 @@
       <c r="Q37" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R37" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -3076,8 +3371,11 @@
       <c r="Q38" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -3117,8 +3415,11 @@
       <c r="Q39" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R39" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3158,8 +3459,11 @@
       <c r="Q40" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R40" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -3199,8 +3503,11 @@
       <c r="Q41" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R41" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>168</v>
       </c>
@@ -3240,8 +3547,11 @@
       <c r="Q42" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -3281,8 +3591,11 @@
       <c r="Q43" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R43" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>194</v>
       </c>
@@ -3322,8 +3635,11 @@
       <c r="Q44" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3363,8 +3679,11 @@
       <c r="Q45" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R45" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -3404,8 +3723,11 @@
       <c r="Q46" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R46" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>132</v>
       </c>
@@ -3457,8 +3779,11 @@
       <c r="Q47" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R47" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>69</v>
       </c>
@@ -3483,8 +3808,11 @@
       <c r="Q48" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R48" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>164</v>
       </c>
@@ -3512,8 +3840,11 @@
       <c r="Q49" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R49" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3541,8 +3872,11 @@
       <c r="Q50" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R50" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -3570,8 +3904,11 @@
       <c r="Q51" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R51" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>114</v>
       </c>
@@ -3596,8 +3933,11 @@
       <c r="Q52" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R52" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>128</v>
       </c>
@@ -3628,8 +3968,11 @@
       <c r="Q53" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R53" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -3660,8 +4003,11 @@
       <c r="Q54" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R54" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -3683,8 +4029,11 @@
       <c r="Q55" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R55" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>90</v>
       </c>
@@ -3706,8 +4055,11 @@
       <c r="Q56" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R56" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -3729,8 +4081,11 @@
       <c r="Q57" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R57" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>196</v>
       </c>
@@ -3752,8 +4107,11 @@
       <c r="Q58" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R58" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>188</v>
       </c>
@@ -3775,8 +4133,11 @@
       <c r="Q59" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R59" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>186</v>
       </c>
@@ -3798,8 +4159,11 @@
       <c r="Q60" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R60" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>28</v>
       </c>
@@ -3820,6 +4184,9 @@
       </c>
       <c r="Q61" t="s">
         <v>221</v>
+      </c>
+      <c r="R61" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>